<commit_message>
set java to 10 version
</commit_message>
<xml_diff>
--- a/src/test/resources/files/testdata.xlsx
+++ b/src/test/resources/files/testdata.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="23">
   <si>
     <t>wwww@test.pl</t>
   </si>
@@ -54,6 +54,54 @@
   </si>
   <si>
     <t>[US-111]/[1] I CAN LOG INTO AUTOMATIONPRACTICE.COM USING REGISTERED EMAIL "THOR.ODINSON@EXAMPLE.COM" &amp; PASSWORD "12345"</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>[POC]/[1]AS A DEVELOPER I'D LIKE TO SEE WORKING POC WITH .XLSX FILE</t>
+  </si>
+  <si>
+    <t>[API]/[1] I WOULD LIKE TO CHECK AVAILABILITY OF AUTOMATIONPRACTICE.COM</t>
+  </si>
+  <si>
+    <t>[US-444]/[1] I WOULD LIKE TO SEE REGISTRATION ERROR, WHEN I DON'T FILL FIRST NAME INPUT</t>
+  </si>
+  <si>
+    <t>[US-555]/[1] I WOULD LIKE TO USE SEARCH BOX AND BE ABLE TO SEE RESULTS OF: "T-SHIRTS"</t>
+  </si>
+  <si>
+    <t>[US-333]/[1] I CHECK AVAILABILITY OF REGISTRATION PAGE FORM</t>
+  </si>
+  <si>
+    <t>[US-666]/[1] I WOULD LIKE TO BUY NEW "FADED SHORT SLEEVE T-SHIRTS"</t>
+  </si>
+  <si>
+    <t>[US-444]/[10] I WOULD LIKE TO SEE REGISTRATION ERROR, WHEN I DON'T FILL MOBILE PHONE INPUT</t>
+  </si>
+  <si>
+    <t>[US-777]/[1] I CLICK ON SOCIAL MEDIA "FACEBOOK" LOGO</t>
+  </si>
+  <si>
+    <t>[US-222]/[1] I AM ABLE TO SEND REQUEST VIA CONTACT US FORM, ALL INPUTS ARE FILLED UP</t>
+  </si>
+  <si>
+    <t>[US-222]/[2] I AM ABLE TO SEND REQUEST VIA CONTACT US FORM, ALL REQUIRED INPUTS ARE FILLED UP</t>
+  </si>
+  <si>
+    <t>[US-444]/[11] I WOULD LIKE TO SEE REGISTRATION ERROR, WHEN I DON'T FILL EMAIL ALIAS INPUT</t>
+  </si>
+  <si>
+    <t>[US-222]/[3] I AM ABLE TO SEND REQUEST VIA CONTACT US FORM WITCH ATTACHED FILE</t>
+  </si>
+  <si>
+    <t>[US-444]/[2] I WOULD LIKE TO SEE REGISTRATION ERROR, WHEN I DON'T FILL LAST NAME INPUT</t>
+  </si>
+  <si>
+    <t>[US-444]/[3] I WOULD LIKE TO SEE REGISTRATION ERROR, WHEN I DON'T FILL EMAIL INPUT</t>
+  </si>
+  <si>
+    <t>[US-222]/[4] I AM NOT ABLE TO SEND REQUEST VIA CONTACT US FORM, EMAIL INPUT IS INVALID</t>
   </si>
 </sst>
 </file>
@@ -1064,11 +1112,15 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" ht="17" thickBot="1">
-      <c r="A46" s="8"/>
+      <c r="A46" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
-      <c r="E46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
       <c r="H46" s="10"/>
@@ -1119,11 +1171,15 @@
       <c r="I50" s="10"/>
     </row>
     <row r="51" spans="1:9" ht="17" thickBot="1">
-      <c r="A51" s="8"/>
+      <c r="A51" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
-      <c r="E51" s="4"/>
+      <c r="E51" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="10"/>

</xml_diff>